<commit_message>
Some test data path updated and alluer report details updated
</commit_message>
<xml_diff>
--- a/TuduApplication/TestData/NewProject.xlsx
+++ b/TuduApplication/TestData/NewProject.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vikesh\Test_projects\TuduApplication\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vikesh\git\NewTUDU\TuduApplication\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DE8DA6-9A8F-4CAF-BF39-570C6959F6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB777F8-8C8D-46AE-B388-E62E9DC95BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E7554D94-690C-4CD3-9D75-8B2892EC350D}"/>
   </bookViews>
@@ -57,7 +57,7 @@
     <t>abc</t>
   </si>
   <si>
-    <t>Vikesh latest project</t>
+    <t>A9 project</t>
   </si>
 </sst>
 </file>

</xml_diff>